<commit_message>
actualización de checklist de auditoria
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Ciclo de vida IWM/5. Aseguramiento de la calidad/PTLL_Auditoria.xlsx
+++ b/Organización/Procesos/Ciclo de vida IWM/5. Aseguramiento de la calidad/PTLL_Auditoria.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="192">
   <si>
     <t>DATOS GENERALES</t>
   </si>
@@ -568,6 +568,66 @@
   </si>
   <si>
     <t>¿Se tiene definido el costo total del desarrollo del proyecto?</t>
+  </si>
+  <si>
+    <t>Analisis y Diseño</t>
+  </si>
+  <si>
+    <t>¿Se definieron objetivos?</t>
+  </si>
+  <si>
+    <t>¿Se definio un alcance?</t>
+  </si>
+  <si>
+    <t>¿Se tiene un analisis?</t>
+  </si>
+  <si>
+    <t>¿Se indentificaron los requerimientos?</t>
+  </si>
+  <si>
+    <t>¿Se definio un diseño de arquitectura?</t>
+  </si>
+  <si>
+    <t>¿Se definio un vista lógica?</t>
+  </si>
+  <si>
+    <t>¿Se definio una vista de desarrollo?</t>
+  </si>
+  <si>
+    <t>¿Se definio una vista de procesos?</t>
+  </si>
+  <si>
+    <t>¿Se definio una vista física?</t>
+  </si>
+  <si>
+    <t>¿Se definieron escenarios?</t>
+  </si>
+  <si>
+    <t>¿Se especifico una estructura de interfaz?</t>
+  </si>
+  <si>
+    <t>Casos de Pruebas</t>
+  </si>
+  <si>
+    <t>¿Se tienen definidos los casos de prueba?</t>
+  </si>
+  <si>
+    <t>¿Cada caso de prueba tiene un caso de uso asociado?</t>
+  </si>
+  <si>
+    <t>¿Se tiene la descripción para cada caso de prueba?</t>
+  </si>
+  <si>
+    <t>¿Se definieron pre condiciones para los casos de prueba?</t>
+  </si>
+  <si>
+    <t>¿Se definieron los pasos para cada caso de prueba?</t>
+  </si>
+  <si>
+    <t>¿Se tienen los datos para los casos de prueba?</t>
+  </si>
+  <si>
+    <t>¿Se tiene un resultado esperado para todos los casos de prueba?</t>
   </si>
 </sst>
 </file>
@@ -1114,6 +1174,21 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1132,31 +1207,16 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1498,10 +1558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1519,76 +1579,76 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
     </row>
     <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="63"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="57"/>
     </row>
     <row r="6" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="55"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="60"/>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="55"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="60"/>
     </row>
     <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="55"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="31" t="s">
@@ -1687,11 +1747,11 @@
     </row>
     <row r="19" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
     </row>
     <row r="21" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="30" t="s">
@@ -1763,185 +1823,213 @@
     <row r="26" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="33" t="str">
         <f>Productos!B68</f>
-        <v>Presentación y Seguimiento</v>
+        <v>Analisis y Diseño</v>
       </c>
       <c r="C26" s="34">
-        <f>COUNTA(Productos!D69:D76)</f>
+        <f>COUNTA(Productos!D69:D79)</f>
         <v>0</v>
       </c>
       <c r="D26" s="35" t="e">
-        <f>COUNTIF((Productos!D69:D76),"x")/(COUNTIF((Productos!D69:D76),"x")+COUNTIF((Productos!E69:E76),"x"))</f>
+        <f>COUNTIF((Productos!D69:D79),"x")/(COUNTIF((Productos!D69:D79),"x")+COUNTIF((Productos!E69:E79),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="33" t="str">
-        <f>Productos!B78</f>
+        <f>Productos!B81</f>
+        <v>Casos de Pruebas</v>
+      </c>
+      <c r="C27" s="34">
+        <f>COUNTA(Productos!D82:D88)</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="35" t="e">
+        <f>COUNTIF((Productos!D82:D88),"x")/(COUNTIF((Productos!D82:D88),"x")+COUNTIF((Productos!E82:E88),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="33" t="str">
+        <f>Productos!B90</f>
+        <v>Presentación y Seguimiento</v>
+      </c>
+      <c r="C28" s="34">
+        <f>COUNTA(Productos!D91:D98)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="35" t="e">
+        <f>COUNTIF((Productos!D91:D98),"x")/(COUNTIF((Productos!D91:D98),"x")+COUNTIF((Productos!E91:E98),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="33" t="str">
+        <f>Productos!B100</f>
         <v>Toma de Decision</v>
       </c>
-      <c r="C27" s="34">
-        <f>COUNTA(Productos!D79:D83)</f>
+      <c r="C29" s="34">
+        <f>COUNTA(Productos!D101:D105)</f>
         <v>0</v>
       </c>
-      <c r="D27" s="35" t="e">
-        <f>COUNTIF((Productos!D79:D83),"x")/(COUNTIF((Productos!D79:D83),"x")+COUNTIF((Productos!E79:E83),"x"))</f>
+      <c r="D29" s="35" t="e">
+        <f>COUNTIF((Productos!D101:D105),"x")/(COUNTIF((Productos!D101:D105),"x")+COUNTIF((Productos!E101:E105),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="2:8" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="57" t="s">
+    <row r="30" spans="2:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:8" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="58"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-    </row>
-    <row r="30" spans="2:8" s="25" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="32" t="s">
+      <c r="C31" s="63"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+    </row>
+    <row r="32" spans="2:8" s="25" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C32" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="32" t="s">
+      <c r="D32" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="23"/>
-    </row>
-    <row r="31" spans="2:8" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="24" t="str">
+      <c r="E32" s="23"/>
+    </row>
+    <row r="33" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="24" t="str">
         <f>Fisica!B4</f>
         <v>Elementos de Configuración</v>
       </c>
-      <c r="C31" s="26">
+      <c r="C33" s="26">
         <f>COUNTA(Fisica!D5:D7)</f>
         <v>0</v>
       </c>
-      <c r="D31" s="27" t="e">
+      <c r="D33" s="27" t="e">
         <f>COUNTIF((Fisica!D5:D7),"x")/(COUNTIF((Fisica!D5:D7),"x")+COUNTIF((Fisica!E5:E7),"x"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E31" s="23"/>
-    </row>
-    <row r="32" spans="2:8" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="24" t="str">
+      <c r="E33" s="23"/>
+    </row>
+    <row r="34" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="24" t="str">
         <f>Fisica!B9</f>
         <v>Línea Base</v>
       </c>
-      <c r="C32" s="26">
+      <c r="C34" s="26">
         <f>COUNTA(Fisica!D10:D13)</f>
         <v>0</v>
       </c>
-      <c r="D32" s="27" t="e">
+      <c r="D34" s="27" t="e">
         <f>COUNTIF((Fisica!D10:D13),"x")/(COUNTIF((Fisica!D10:D13),"x")+COUNTIF((Fisica!E10:E13),"x"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E32" s="23"/>
-    </row>
-    <row r="33" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="24" t="str">
+      <c r="E34" s="23"/>
+    </row>
+    <row r="35" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="24" t="str">
         <f>Fisica!B15</f>
         <v>Control de Cambios</v>
       </c>
-      <c r="C33" s="26">
+      <c r="C35" s="26">
         <f>COUNTA(Fisica!D16:D16)</f>
         <v>0</v>
       </c>
-      <c r="D33" s="27" t="e">
+      <c r="D35" s="27" t="e">
         <f>COUNTIF((Fisica!D16:D16),"x")/(COUNTIF((Fisica!D16:D16),"x")+COUNTIF((Fisica!E16:E16),"x"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E33" s="23"/>
-    </row>
-    <row r="34" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="56" t="s">
+      <c r="E35" s="23"/>
+    </row>
+    <row r="36" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="28"/>
-    </row>
-    <row r="36" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="31" t="s">
+      <c r="C37" s="61"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="28"/>
+    </row>
+    <row r="38" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="31" t="s">
+      <c r="C38" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D36" s="31" t="s">
+      <c r="D38" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E36" s="28"/>
-    </row>
-    <row r="37" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="33" t="str">
+      <c r="E38" s="28"/>
+    </row>
+    <row r="39" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="33" t="str">
         <f>Funcional!B4</f>
         <v>Líneas Base</v>
       </c>
-      <c r="C37" s="34">
+      <c r="C39" s="34">
         <f>COUNTA(Funcional!D5:D8)</f>
         <v>0</v>
       </c>
-      <c r="D37" s="35" t="e">
+      <c r="D39" s="35" t="e">
         <f>COUNTIF((Funcional!D5:D8),"x")/(COUNTIF((Funcional!D5:D8),"x")+COUNTIF((Funcional!E5:E8),"x"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E37" s="28"/>
-    </row>
-    <row r="38" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="33" t="str">
+      <c r="E39" s="28"/>
+    </row>
+    <row r="40" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="33" t="str">
         <f>Funcional!B10</f>
         <v>Entregables</v>
       </c>
-      <c r="C38" s="34">
+      <c r="C40" s="34">
         <f>COUNTA(Funcional!D11:D18)</f>
         <v>0</v>
       </c>
-      <c r="D38" s="35" t="e">
+      <c r="D40" s="35" t="e">
         <f>COUNTIF((Funcional!D11:D18),"x")/(COUNTIF((Funcional!D11:D18),"x")+COUNTIF((Funcional!E11:E18),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="39" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="33" t="str">
+    <row r="41" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="33" t="str">
         <f>Funcional!B20</f>
         <v>Control de Cambios</v>
       </c>
-      <c r="C39" s="34">
+      <c r="C41" s="34">
         <f>COUNTA(Funcional!D21:D25)</f>
         <v>0</v>
       </c>
-      <c r="D39" s="35" t="e">
+      <c r="D41" s="35" t="e">
         <f>COUNTIF((Funcional!D21:D25),"x")/(COUNTIF((Funcional!D21:D25),"x")+COUNTIF((Funcional!E21:E25),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B31:D31"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B29:D29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="D33" evalError="1"/>
+    <ignoredError sqref="D35" evalError="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1973,22 +2061,22 @@
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66" t="s">
+      <c r="C2" s="64"/>
+      <c r="D2" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66" t="s">
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
       <c r="D3" s="43" t="s">
         <v>5</v>
       </c>
@@ -1998,17 +2086,17 @@
       <c r="F3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="66"/>
+      <c r="G3" s="64"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="10">
@@ -2094,10 +2182,10 @@
         <v>30</v>
       </c>
       <c r="C12" s="69"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
@@ -2250,10 +2338,10 @@
         <v>63</v>
       </c>
       <c r="C25" s="69"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="64"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="10">
@@ -2367,10 +2455,10 @@
       <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="65" t="s">
+      <c r="B35" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="65"/>
+      <c r="C35" s="66"/>
       <c r="D35" s="44"/>
       <c r="E35" s="44"/>
       <c r="F35" s="44"/>
@@ -2402,14 +2490,14 @@
       <c r="G37" s="13"/>
     </row>
     <row r="39" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="65" t="s">
+      <c r="B39" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="65"/>
-      <c r="D39" s="65"/>
-      <c r="E39" s="65"/>
-      <c r="F39" s="65"/>
-      <c r="G39" s="65"/>
+      <c r="C39" s="66"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="66"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="10">
@@ -2506,14 +2594,14 @@
       <c r="C47" s="40"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="65" t="s">
+      <c r="B48" s="66" t="s">
         <v>140</v>
       </c>
-      <c r="C48" s="65"/>
-      <c r="D48" s="65"/>
-      <c r="E48" s="65"/>
-      <c r="F48" s="65"/>
-      <c r="G48" s="65"/>
+      <c r="C48" s="66"/>
+      <c r="D48" s="66"/>
+      <c r="E48" s="66"/>
+      <c r="F48" s="66"/>
+      <c r="G48" s="66"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="10">
@@ -2568,6 +2656,10 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B2:C3"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="D39:E39"/>
@@ -2583,10 +2675,6 @@
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="F25:G25"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <conditionalFormatting sqref="D24:F24 D26:F34">
     <cfRule type="expression" dxfId="2" priority="8" stopIfTrue="1">
@@ -2605,10 +2693,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2633,22 +2721,22 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="70"/>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66" t="s">
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="70"/>
-      <c r="C3" s="66"/>
+      <c r="C3" s="64"/>
       <c r="D3" s="43" t="s">
         <v>5</v>
       </c>
@@ -2658,18 +2746,18 @@
       <c r="F3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="66"/>
+      <c r="G3" s="64"/>
     </row>
     <row r="4" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
     </row>
     <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
@@ -2821,14 +2909,14 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="67" t="s">
         <v>123</v>
       </c>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
@@ -3064,14 +3152,14 @@
     </row>
     <row r="34" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
-      <c r="B34" s="64" t="s">
+      <c r="B34" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="64"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
-      <c r="F34" s="64"/>
-      <c r="G34" s="64"/>
+      <c r="C34" s="67"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="67"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
@@ -3181,14 +3269,14 @@
     </row>
     <row r="43" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
-      <c r="B43" s="64" t="s">
+      <c r="B43" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="64"/>
-      <c r="D43" s="64"/>
-      <c r="E43" s="64"/>
-      <c r="F43" s="64"/>
-      <c r="G43" s="64"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="67"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
@@ -3520,23 +3608,24 @@
       <c r="F67" s="48"/>
       <c r="G67" s="48"/>
     </row>
-    <row r="68" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
-      <c r="B68" s="64" t="s">
-        <v>62</v>
-      </c>
-      <c r="C68" s="64"/>
-      <c r="D68" s="64"/>
-      <c r="E68" s="64"/>
-      <c r="F68" s="64"/>
-      <c r="G68" s="64"/>
+      <c r="B68" s="67" t="s">
+        <v>172</v>
+      </c>
+      <c r="C68" s="67"/>
+      <c r="D68" s="67"/>
+      <c r="E68" s="67"/>
+      <c r="F68" s="67"/>
+      <c r="G68" s="67"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B69" s="10">
+      <c r="A69" s="5"/>
+      <c r="B69" s="48">
         <v>1</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>127</v>
+        <v>173</v>
       </c>
       <c r="D69" s="12"/>
       <c r="E69" s="12"/>
@@ -3544,12 +3633,13 @@
       <c r="G69" s="13"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B70" s="10">
+      <c r="A70" s="5"/>
+      <c r="B70" s="48">
         <f>B69+1</f>
         <v>2</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>128</v>
+        <v>174</v>
       </c>
       <c r="D70" s="12"/>
       <c r="E70" s="12"/>
@@ -3557,12 +3647,13 @@
       <c r="G70" s="13"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="10">
-        <f t="shared" ref="B71:B76" si="4">B70+1</f>
+      <c r="A71" s="5"/>
+      <c r="B71" s="48">
+        <f t="shared" ref="B71:B79" si="4">B70+1</f>
         <v>3</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>129</v>
+        <v>175</v>
       </c>
       <c r="D71" s="12"/>
       <c r="E71" s="12"/>
@@ -3570,12 +3661,13 @@
       <c r="G71" s="13"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B72" s="10">
+      <c r="A72" s="5"/>
+      <c r="B72" s="48">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>130</v>
+        <v>176</v>
       </c>
       <c r="D72" s="12"/>
       <c r="E72" s="12"/>
@@ -3583,12 +3675,13 @@
       <c r="G72" s="13"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B73" s="10">
+      <c r="A73" s="5"/>
+      <c r="B73" s="48">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>131</v>
+        <v>177</v>
       </c>
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
@@ -3596,12 +3689,13 @@
       <c r="G73" s="13"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B74" s="10">
+      <c r="A74" s="5"/>
+      <c r="B74" s="48">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>132</v>
+        <v>178</v>
       </c>
       <c r="D74" s="12"/>
       <c r="E74" s="12"/>
@@ -3609,12 +3703,13 @@
       <c r="G74" s="13"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B75" s="10">
+      <c r="A75" s="5"/>
+      <c r="B75" s="48">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>133</v>
+        <v>180</v>
       </c>
       <c r="D75" s="12"/>
       <c r="E75" s="12"/>
@@ -3622,12 +3717,13 @@
       <c r="G75" s="13"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B76" s="10">
+      <c r="A76" s="5"/>
+      <c r="B76" s="48">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>134</v>
+        <v>179</v>
       </c>
       <c r="D76" s="12"/>
       <c r="E76" s="12"/>
@@ -3635,24 +3731,41 @@
       <c r="G76" s="13"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C77" s="20"/>
+      <c r="A77" s="5"/>
+      <c r="B77" s="48">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="13"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B78" s="64" t="s">
-        <v>145</v>
-      </c>
-      <c r="C78" s="64"/>
-      <c r="D78" s="64"/>
-      <c r="E78" s="64"/>
-      <c r="F78" s="64"/>
-      <c r="G78" s="64"/>
+      <c r="A78" s="5"/>
+      <c r="B78" s="48">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="13"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B79" s="10">
-        <v>1</v>
+      <c r="A79" s="5"/>
+      <c r="B79" s="48">
+        <f t="shared" si="4"/>
+        <v>11</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
       <c r="D79" s="12"/>
       <c r="E79" s="12"/>
@@ -3660,59 +3773,336 @@
       <c r="G79" s="13"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="10">
-        <f>B79+1</f>
-        <v>2</v>
-      </c>
-      <c r="C80" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
-      <c r="G80" s="13"/>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B81" s="10">
-        <f t="shared" ref="B81:B83" si="5">B80+1</f>
-        <v>3</v>
-      </c>
-      <c r="C81" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="D81" s="12"/>
-      <c r="E81" s="12"/>
-      <c r="F81" s="12"/>
-      <c r="G81" s="13"/>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B82" s="10">
-        <f t="shared" si="5"/>
-        <v>4</v>
+      <c r="A80" s="5"/>
+      <c r="B80" s="48"/>
+      <c r="C80" s="48"/>
+      <c r="D80" s="48"/>
+      <c r="E80" s="48"/>
+      <c r="F80" s="48"/>
+      <c r="G80" s="48"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="5"/>
+      <c r="B81" s="67" t="s">
+        <v>184</v>
+      </c>
+      <c r="C81" s="67"/>
+      <c r="D81" s="67"/>
+      <c r="E81" s="67"/>
+      <c r="F81" s="67"/>
+      <c r="G81" s="67"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="5"/>
+      <c r="B82" s="48">
+        <v>1</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="D82" s="12"/>
       <c r="E82" s="12"/>
       <c r="F82" s="12"/>
       <c r="G82" s="13"/>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B83" s="10">
-        <f t="shared" si="5"/>
-        <v>5</v>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="5"/>
+      <c r="B83" s="48">
+        <f>B82+1</f>
+        <v>2</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="D83" s="12"/>
       <c r="E83" s="12"/>
       <c r="F83" s="12"/>
       <c r="G83" s="13"/>
     </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="5"/>
+      <c r="B84" s="48">
+        <f t="shared" ref="B84:B88" si="5">B83+1</f>
+        <v>3</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="13"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="5"/>
+      <c r="B85" s="48">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="13"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="5"/>
+      <c r="B86" s="48">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="12"/>
+      <c r="G86" s="13"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="5"/>
+      <c r="B87" s="48">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D87" s="12"/>
+      <c r="E87" s="12"/>
+      <c r="F87" s="12"/>
+      <c r="G87" s="13"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="5"/>
+      <c r="B88" s="48">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+      <c r="G88" s="13"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="5"/>
+      <c r="B89" s="48"/>
+      <c r="C89" s="48"/>
+      <c r="D89" s="48"/>
+      <c r="E89" s="48"/>
+      <c r="F89" s="48"/>
+      <c r="G89" s="48"/>
+    </row>
+    <row r="90" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="5"/>
+      <c r="B90" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="C90" s="67"/>
+      <c r="D90" s="67"/>
+      <c r="E90" s="67"/>
+      <c r="F90" s="67"/>
+      <c r="G90" s="67"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="10">
+        <v>1</v>
+      </c>
+      <c r="C91" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="13"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="10">
+        <f>B91+1</f>
+        <v>2</v>
+      </c>
+      <c r="C92" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12"/>
+      <c r="G92" s="13"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="10">
+        <f t="shared" ref="B93:B98" si="6">B92+1</f>
+        <v>3</v>
+      </c>
+      <c r="C93" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D93" s="12"/>
+      <c r="E93" s="12"/>
+      <c r="F93" s="12"/>
+      <c r="G93" s="13"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B94" s="10">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="C94" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12"/>
+      <c r="G94" s="13"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B95" s="10">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="C95" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
+      <c r="G95" s="13"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B96" s="10">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D96" s="12"/>
+      <c r="E96" s="12"/>
+      <c r="F96" s="12"/>
+      <c r="G96" s="13"/>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97" s="10">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D97" s="12"/>
+      <c r="E97" s="12"/>
+      <c r="F97" s="12"/>
+      <c r="G97" s="13"/>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B98" s="10">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="C98" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="13"/>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C99" s="20"/>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100" s="67" t="s">
+        <v>145</v>
+      </c>
+      <c r="C100" s="67"/>
+      <c r="D100" s="67"/>
+      <c r="E100" s="67"/>
+      <c r="F100" s="67"/>
+      <c r="G100" s="67"/>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B101" s="10">
+        <v>1</v>
+      </c>
+      <c r="C101" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D101" s="12"/>
+      <c r="E101" s="12"/>
+      <c r="F101" s="12"/>
+      <c r="G101" s="13"/>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B102" s="10">
+        <f>B101+1</f>
+        <v>2</v>
+      </c>
+      <c r="C102" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D102" s="12"/>
+      <c r="E102" s="12"/>
+      <c r="F102" s="12"/>
+      <c r="G102" s="13"/>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B103" s="10">
+        <f t="shared" ref="B103:B105" si="7">B102+1</f>
+        <v>3</v>
+      </c>
+      <c r="C103" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D103" s="12"/>
+      <c r="E103" s="12"/>
+      <c r="F103" s="12"/>
+      <c r="G103" s="13"/>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B104" s="10">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="C104" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D104" s="12"/>
+      <c r="E104" s="12"/>
+      <c r="F104" s="12"/>
+      <c r="G104" s="13"/>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B105" s="10">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="C105" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D105" s="12"/>
+      <c r="E105" s="12"/>
+      <c r="F105" s="12"/>
+      <c r="G105" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="28">
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="F100:G100"/>
+    <mergeCell ref="B90:C90"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B34:C34"/>
@@ -3729,14 +4119,8 @@
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="F43:G43"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="B68:C68"/>
   </mergeCells>
-  <conditionalFormatting sqref="C77">
+  <conditionalFormatting sqref="C99">
     <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
       <formula>IF(#REF!,TRUE,FALSE)</formula>
     </cfRule>
@@ -3769,16 +4153,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66" t="s">
+      <c r="C2" s="64"/>
+      <c r="D2" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66" t="s">
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="4"/>
@@ -3799,7 +4183,7 @@
       <c r="F3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="66"/>
+      <c r="G3" s="64"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -3807,14 +4191,14 @@
       <c r="L3" s="4"/>
     </row>
     <row r="4" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="67" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -3894,14 +4278,14 @@
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
       <c r="H9" s="4"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -4000,14 +4384,14 @@
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
       <c r="H15" s="4"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -4043,6 +4427,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="B15:C15"/>
@@ -4050,11 +4439,6 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
@@ -4082,22 +4466,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66" t="s">
+      <c r="C2" s="64"/>
+      <c r="D2" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66" t="s">
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
       <c r="D3" s="43" t="s">
         <v>5</v>
       </c>
@@ -4107,17 +4491,17 @@
       <c r="F3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="66"/>
+      <c r="G3" s="64"/>
     </row>
     <row r="4" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="10">
@@ -4176,14 +4560,14 @@
       <c r="G9" s="48"/>
     </row>
     <row r="10" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="67"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
@@ -4292,14 +4676,14 @@
       <c r="G19" s="48"/>
     </row>
     <row r="20" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="64" t="s">
+      <c r="B20" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
@@ -4386,18 +4770,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <Status xmlns="035E5738-9077-49AA-867C-265905AEBD06">Final</Status>
-    <Owner xmlns="035E5738-9077-49AA-867C-265905AEBD06">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4485,25 +4863,24 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <Status xmlns="035E5738-9077-49AA-867C-265905AEBD06">Final</Status>
+    <Owner xmlns="035E5738-9077-49AA-867C-265905AEBD06">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B74BF6BA-412C-41A7-B0A7-7E1FCDB78793}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4BF54FE-89ED-4BFD-984C-5255D8E3B158}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4526,9 +4903,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4BF54FE-89ED-4BFD-984C-5255D8E3B158}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B74BF6BA-412C-41A7-B0A7-7E1FCDB78793}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Se actualizo el checklist en la pestaña de producto
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Ciclo de vida IWM/5. Aseguramiento de la calidad/PTLL_Auditoria.xlsx
+++ b/Organización/Procesos/Ciclo de vida IWM/5. Aseguramiento de la calidad/PTLL_Auditoria.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="197">
   <si>
     <t>DATOS GENERALES</t>
   </si>
@@ -628,6 +628,21 @@
   </si>
   <si>
     <t>¿Se tiene un resultado esperado para todos los casos de prueba?</t>
+  </si>
+  <si>
+    <t>Entrega Proyecto</t>
+  </si>
+  <si>
+    <t>¿Se tiene el nombre de contacto del cliente?</t>
+  </si>
+  <si>
+    <t>¿Se tiene el nombre de la empresa a quien se desarrollo el proyecto?</t>
+  </si>
+  <si>
+    <t>¿Se tiene la lista de documentos a entregar?</t>
+  </si>
+  <si>
+    <t>¿Se tiene firmado el documento de entrega?</t>
   </si>
 </sst>
 </file>
@@ -1174,6 +1189,24 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1189,32 +1222,14 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1558,10 +1573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1579,76 +1594,76 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
     </row>
     <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="57"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="63"/>
     </row>
     <row r="6" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="60"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="55"/>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="60"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="55"/>
     </row>
     <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="58" t="s">
+      <c r="C8" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="55"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="31" t="s">
@@ -1747,11 +1762,11 @@
     </row>
     <row r="19" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
     </row>
     <row r="21" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="30" t="s">
@@ -1851,185 +1866,199 @@
     <row r="28" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="33" t="str">
         <f>Productos!B90</f>
-        <v>Presentación y Seguimiento</v>
+        <v>Entrega Proyecto</v>
       </c>
       <c r="C28" s="34">
-        <f>COUNTA(Productos!D91:D98)</f>
+        <f>COUNTA(Productos!D91:D94)</f>
         <v>0</v>
       </c>
       <c r="D28" s="35" t="e">
-        <f>COUNTIF((Productos!D91:D98),"x")/(COUNTIF((Productos!D91:D98),"x")+COUNTIF((Productos!E91:E98),"x"))</f>
+        <f>COUNTIF((Productos!D91:D94),"x")/(COUNTIF((Productos!D91:D94),"x")+COUNTIF((Productos!E91:E94),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="33" t="str">
-        <f>Productos!B100</f>
+        <f>Productos!B96</f>
+        <v>Presentación y Seguimiento</v>
+      </c>
+      <c r="C29" s="34">
+        <f>COUNTA(Productos!D97:D104)</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="35" t="e">
+        <f>COUNTIF((Productos!D97:D104),"x")/(COUNTIF((Productos!D97:D104),"x")+COUNTIF((Productos!E97:E104),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="33" t="str">
+        <f>Productos!B106</f>
         <v>Toma de Decision</v>
       </c>
-      <c r="C29" s="34">
-        <f>COUNTA(Productos!D101:D105)</f>
+      <c r="C30" s="34">
+        <f>COUNTA(Productos!D107:D111)</f>
         <v>0</v>
       </c>
-      <c r="D29" s="35" t="e">
-        <f>COUNTIF((Productos!D101:D105),"x")/(COUNTIF((Productos!D101:D105),"x")+COUNTIF((Productos!E101:E105),"x"))</f>
+      <c r="D30" s="35" t="e">
+        <f>COUNTIF((Productos!D107:D111),"x")/(COUNTIF((Productos!D107:D111),"x")+COUNTIF((Productos!E107:E111),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:8" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="62" t="s">
+    <row r="31" spans="2:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="2:8" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="63"/>
-      <c r="D31" s="63"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-    </row>
-    <row r="32" spans="2:8" s="25" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="32" t="s">
+      <c r="C32" s="58"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+    </row>
+    <row r="33" spans="2:5" s="25" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C33" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="32" t="s">
+      <c r="D33" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="23"/>
-    </row>
-    <row r="33" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="24" t="str">
+      <c r="E33" s="23"/>
+    </row>
+    <row r="34" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="24" t="str">
         <f>Fisica!B4</f>
         <v>Elementos de Configuración</v>
       </c>
-      <c r="C33" s="26">
+      <c r="C34" s="26">
         <f>COUNTA(Fisica!D5:D7)</f>
         <v>0</v>
       </c>
-      <c r="D33" s="27" t="e">
+      <c r="D34" s="27" t="e">
         <f>COUNTIF((Fisica!D5:D7),"x")/(COUNTIF((Fisica!D5:D7),"x")+COUNTIF((Fisica!E5:E7),"x"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E33" s="23"/>
-    </row>
-    <row r="34" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="24" t="str">
+      <c r="E34" s="23"/>
+    </row>
+    <row r="35" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="24" t="str">
         <f>Fisica!B9</f>
         <v>Línea Base</v>
       </c>
-      <c r="C34" s="26">
+      <c r="C35" s="26">
         <f>COUNTA(Fisica!D10:D13)</f>
         <v>0</v>
       </c>
-      <c r="D34" s="27" t="e">
+      <c r="D35" s="27" t="e">
         <f>COUNTIF((Fisica!D10:D13),"x")/(COUNTIF((Fisica!D10:D13),"x")+COUNTIF((Fisica!E10:E13),"x"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E34" s="23"/>
-    </row>
-    <row r="35" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="24" t="str">
+      <c r="E35" s="23"/>
+    </row>
+    <row r="36" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="24" t="str">
         <f>Fisica!B15</f>
         <v>Control de Cambios</v>
       </c>
-      <c r="C35" s="26">
+      <c r="C36" s="26">
         <f>COUNTA(Fisica!D16:D16)</f>
         <v>0</v>
       </c>
-      <c r="D35" s="27" t="e">
+      <c r="D36" s="27" t="e">
         <f>COUNTIF((Fisica!D16:D16),"x")/(COUNTIF((Fisica!D16:D16),"x")+COUNTIF((Fisica!E16:E16),"x"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E35" s="23"/>
-    </row>
-    <row r="36" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="61" t="s">
+      <c r="E36" s="23"/>
+    </row>
+    <row r="37" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="61"/>
-      <c r="D37" s="61"/>
-      <c r="E37" s="28"/>
-    </row>
-    <row r="38" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="31" t="s">
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="28"/>
+    </row>
+    <row r="39" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="31" t="s">
+      <c r="C39" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D38" s="31" t="s">
+      <c r="D39" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="28"/>
-    </row>
-    <row r="39" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="33" t="str">
+      <c r="E39" s="28"/>
+    </row>
+    <row r="40" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="33" t="str">
         <f>Funcional!B4</f>
         <v>Líneas Base</v>
       </c>
-      <c r="C39" s="34">
+      <c r="C40" s="34">
         <f>COUNTA(Funcional!D5:D8)</f>
         <v>0</v>
       </c>
-      <c r="D39" s="35" t="e">
+      <c r="D40" s="35" t="e">
         <f>COUNTIF((Funcional!D5:D8),"x")/(COUNTIF((Funcional!D5:D8),"x")+COUNTIF((Funcional!E5:E8),"x"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E39" s="28"/>
-    </row>
-    <row r="40" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="33" t="str">
+      <c r="E40" s="28"/>
+    </row>
+    <row r="41" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="33" t="str">
         <f>Funcional!B10</f>
         <v>Entregables</v>
       </c>
-      <c r="C40" s="34">
+      <c r="C41" s="34">
         <f>COUNTA(Funcional!D11:D18)</f>
         <v>0</v>
       </c>
-      <c r="D40" s="35" t="e">
+      <c r="D41" s="35" t="e">
         <f>COUNTIF((Funcional!D11:D18),"x")/(COUNTIF((Funcional!D11:D18),"x")+COUNTIF((Funcional!E11:E18),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="33" t="str">
+    <row r="42" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="33" t="str">
         <f>Funcional!B20</f>
         <v>Control de Cambios</v>
       </c>
-      <c r="C41" s="34">
+      <c r="C42" s="34">
         <f>COUNTA(Funcional!D21:D25)</f>
         <v>0</v>
       </c>
-      <c r="D41" s="35" t="e">
+      <c r="D42" s="35" t="e">
         <f>COUNTIF((Funcional!D21:D25),"x")/(COUNTIF((Funcional!D21:D25),"x")+COUNTIF((Funcional!E21:E25),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B31:D31"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B32:D32"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="D35" evalError="1"/>
+    <ignoredError sqref="D36" evalError="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2061,22 +2090,22 @@
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64" t="s">
+      <c r="C2" s="65"/>
+      <c r="D2" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64" t="s">
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
       <c r="D3" s="43" t="s">
         <v>5</v>
       </c>
@@ -2086,7 +2115,7 @@
       <c r="F3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="64"/>
+      <c r="G3" s="65"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="67" t="s">
@@ -2455,10 +2484,10 @@
       <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="66" t="s">
+      <c r="B35" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="66"/>
+      <c r="C35" s="64"/>
       <c r="D35" s="44"/>
       <c r="E35" s="44"/>
       <c r="F35" s="44"/>
@@ -2490,14 +2519,14 @@
       <c r="G37" s="13"/>
     </row>
     <row r="39" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="66" t="s">
+      <c r="B39" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="66"/>
-      <c r="D39" s="66"/>
-      <c r="E39" s="66"/>
-      <c r="F39" s="66"/>
-      <c r="G39" s="66"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="64"/>
+      <c r="G39" s="64"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="10">
@@ -2594,14 +2623,14 @@
       <c r="C47" s="40"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="66" t="s">
+      <c r="B48" s="64" t="s">
         <v>140</v>
       </c>
-      <c r="C48" s="66"/>
-      <c r="D48" s="66"/>
-      <c r="E48" s="66"/>
-      <c r="F48" s="66"/>
-      <c r="G48" s="66"/>
+      <c r="C48" s="64"/>
+      <c r="D48" s="64"/>
+      <c r="E48" s="64"/>
+      <c r="F48" s="64"/>
+      <c r="G48" s="64"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="10">
@@ -2656,6 +2685,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="F48:G48"/>
@@ -2672,9 +2704,6 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
   </mergeCells>
   <conditionalFormatting sqref="D24:F24 D26:F34">
     <cfRule type="expression" dxfId="2" priority="8" stopIfTrue="1">
@@ -2693,10 +2722,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G105"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2721,22 +2750,22 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="70"/>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64" t="s">
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="70"/>
-      <c r="C3" s="64"/>
+      <c r="C3" s="65"/>
       <c r="D3" s="43" t="s">
         <v>5</v>
       </c>
@@ -2746,7 +2775,7 @@
       <c r="F3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="64"/>
+      <c r="G3" s="65"/>
     </row>
     <row r="4" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -3898,10 +3927,10 @@
       <c r="F89" s="48"/>
       <c r="G89" s="48"/>
     </row>
-    <row r="90" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
       <c r="B90" s="67" t="s">
-        <v>62</v>
+        <v>192</v>
       </c>
       <c r="C90" s="67"/>
       <c r="D90" s="67"/>
@@ -3910,11 +3939,12 @@
       <c r="G90" s="67"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B91" s="10">
+      <c r="A91" s="5"/>
+      <c r="B91" s="48">
         <v>1</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>127</v>
+        <v>193</v>
       </c>
       <c r="D91" s="12"/>
       <c r="E91" s="12"/>
@@ -3922,12 +3952,13 @@
       <c r="G91" s="13"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B92" s="10">
+      <c r="A92" s="5"/>
+      <c r="B92" s="48">
         <f>B91+1</f>
         <v>2</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>128</v>
+        <v>194</v>
       </c>
       <c r="D92" s="12"/>
       <c r="E92" s="12"/>
@@ -3935,12 +3966,13 @@
       <c r="G92" s="13"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B93" s="10">
-        <f t="shared" ref="B93:B98" si="6">B92+1</f>
+      <c r="A93" s="5"/>
+      <c r="B93" s="48">
+        <f t="shared" ref="B93:B94" si="6">B92+1</f>
         <v>3</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>129</v>
+        <v>195</v>
       </c>
       <c r="D93" s="12"/>
       <c r="E93" s="12"/>
@@ -3948,12 +3980,13 @@
       <c r="G93" s="13"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B94" s="10">
+      <c r="A94" s="5"/>
+      <c r="B94" s="48">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>130</v>
+        <v>196</v>
       </c>
       <c r="D94" s="12"/>
       <c r="E94" s="12"/>
@@ -3961,38 +3994,31 @@
       <c r="G94" s="13"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B95" s="10">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="C95" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="D95" s="12"/>
-      <c r="E95" s="12"/>
-      <c r="F95" s="12"/>
-      <c r="G95" s="13"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B96" s="10">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="C96" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="D96" s="12"/>
-      <c r="E96" s="12"/>
-      <c r="F96" s="12"/>
-      <c r="G96" s="13"/>
+      <c r="A95" s="5"/>
+      <c r="B95" s="48"/>
+      <c r="C95" s="48"/>
+      <c r="D95" s="48"/>
+      <c r="E95" s="48"/>
+      <c r="F95" s="48"/>
+      <c r="G95" s="48"/>
+    </row>
+    <row r="96" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="5"/>
+      <c r="B96" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="C96" s="67"/>
+      <c r="D96" s="67"/>
+      <c r="E96" s="67"/>
+      <c r="F96" s="67"/>
+      <c r="G96" s="67"/>
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97" s="10">
-        <f t="shared" si="6"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D97" s="12"/>
       <c r="E97" s="12"/>
@@ -4001,11 +4027,11 @@
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" s="10">
-        <f t="shared" si="6"/>
-        <v>8</v>
+        <f>B97+1</f>
+        <v>2</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D98" s="12"/>
       <c r="E98" s="12"/>
@@ -4013,24 +4039,38 @@
       <c r="G98" s="13"/>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C99" s="20"/>
+      <c r="B99" s="10">
+        <f t="shared" ref="B99:B104" si="7">B98+1</f>
+        <v>3</v>
+      </c>
+      <c r="C99" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D99" s="12"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="13"/>
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B100" s="67" t="s">
-        <v>145</v>
-      </c>
-      <c r="C100" s="67"/>
-      <c r="D100" s="67"/>
-      <c r="E100" s="67"/>
-      <c r="F100" s="67"/>
-      <c r="G100" s="67"/>
+      <c r="B100" s="10">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="C100" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D100" s="12"/>
+      <c r="E100" s="12"/>
+      <c r="F100" s="12"/>
+      <c r="G100" s="13"/>
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B101" s="10">
-        <v>1</v>
+        <f t="shared" si="7"/>
+        <v>5</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="D101" s="12"/>
       <c r="E101" s="12"/>
@@ -4039,11 +4079,11 @@
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B102" s="10">
-        <f>B101+1</f>
-        <v>2</v>
+        <f t="shared" si="7"/>
+        <v>6</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="D102" s="12"/>
       <c r="E102" s="12"/>
@@ -4052,11 +4092,11 @@
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103" s="10">
-        <f t="shared" ref="B103:B105" si="7">B102+1</f>
-        <v>3</v>
+        <f t="shared" si="7"/>
+        <v>7</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="D103" s="12"/>
       <c r="E103" s="12"/>
@@ -4066,10 +4106,10 @@
     <row r="104" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B104" s="10">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="D104" s="12"/>
       <c r="E104" s="12"/>
@@ -4077,32 +4117,87 @@
       <c r="G104" s="13"/>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B105" s="10">
-        <f t="shared" si="7"/>
+      <c r="C105" s="20"/>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B106" s="67" t="s">
+        <v>145</v>
+      </c>
+      <c r="C106" s="67"/>
+      <c r="D106" s="67"/>
+      <c r="E106" s="67"/>
+      <c r="F106" s="67"/>
+      <c r="G106" s="67"/>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B107" s="10">
+        <v>1</v>
+      </c>
+      <c r="C107" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D107" s="12"/>
+      <c r="E107" s="12"/>
+      <c r="F107" s="12"/>
+      <c r="G107" s="13"/>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B108" s="10">
+        <f>B107+1</f>
+        <v>2</v>
+      </c>
+      <c r="C108" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D108" s="12"/>
+      <c r="E108" s="12"/>
+      <c r="F108" s="12"/>
+      <c r="G108" s="13"/>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B109" s="10">
+        <f t="shared" ref="B109:B111" si="8">B108+1</f>
+        <v>3</v>
+      </c>
+      <c r="C109" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D109" s="12"/>
+      <c r="E109" s="12"/>
+      <c r="F109" s="12"/>
+      <c r="G109" s="13"/>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B110" s="10">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="C110" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D110" s="12"/>
+      <c r="E110" s="12"/>
+      <c r="F110" s="12"/>
+      <c r="G110" s="13"/>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B111" s="10">
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="C105" s="11" t="s">
+      <c r="C111" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="D105" s="12"/>
-      <c r="E105" s="12"/>
-      <c r="F105" s="12"/>
-      <c r="G105" s="13"/>
+      <c r="D111" s="12"/>
+      <c r="E111" s="12"/>
+      <c r="F111" s="12"/>
+      <c r="G111" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="F81:G81"/>
+  <mergeCells count="31">
+    <mergeCell ref="B90:C90"/>
     <mergeCell ref="D90:E90"/>
     <mergeCell ref="F90:G90"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="F100:G100"/>
-    <mergeCell ref="B90:C90"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B34:C34"/>
@@ -4119,8 +4214,20 @@
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="F43:G43"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="F96:G96"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="F106:G106"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="F81:G81"/>
   </mergeCells>
-  <conditionalFormatting sqref="C99">
+  <conditionalFormatting sqref="C105">
     <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
       <formula>IF(#REF!,TRUE,FALSE)</formula>
     </cfRule>
@@ -4153,16 +4260,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64" t="s">
+      <c r="C2" s="65"/>
+      <c r="D2" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64" t="s">
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="4"/>
@@ -4183,7 +4290,7 @@
       <c r="F3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="64"/>
+      <c r="G3" s="65"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -4427,11 +4534,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="B15:C15"/>
@@ -4439,6 +4541,11 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
@@ -4466,22 +4573,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64" t="s">
+      <c r="C2" s="65"/>
+      <c r="D2" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64" t="s">
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
       <c r="D3" s="43" t="s">
         <v>5</v>
       </c>
@@ -4491,7 +4598,7 @@
       <c r="F3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="64"/>
+      <c r="G3" s="65"/>
     </row>
     <row r="4" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="67" t="s">
@@ -4770,12 +4877,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <Status xmlns="035E5738-9077-49AA-867C-265905AEBD06">Final</Status>
+    <Owner xmlns="035E5738-9077-49AA-867C-265905AEBD06">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4863,24 +4976,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <Status xmlns="035E5738-9077-49AA-867C-265905AEBD06">Final</Status>
-    <Owner xmlns="035E5738-9077-49AA-867C-265905AEBD06">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4BF54FE-89ED-4BFD-984C-5255D8E3B158}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B74BF6BA-412C-41A7-B0A7-7E1FCDB78793}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4903,16 +5017,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B74BF6BA-412C-41A7-B0A7-7E1FCDB78793}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4BF54FE-89ED-4BFD-984C-5255D8E3B158}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>